<commit_message>
Figure bioregion boxplot made and smaller updates made to boxplot for method and fishing status.
</commit_message>
<xml_diff>
--- a/Tables/UNI_PERM_Biomass_Boxplot.xlsx
+++ b/Tables/UNI_PERM_Biomass_Boxplot.xlsx
@@ -398,7 +398,7 @@
         <v>0.0465828837782763</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0081</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="3">
@@ -418,7 +418,7 @@
         <v>0.000774333199317747</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7411</v>
+        <v>0.7304</v>
       </c>
     </row>
     <row r="4">
@@ -438,7 +438,7 @@
         <v>0.001561685137529</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6343</v>
+        <v>0.6368</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Cleaning code down to boxplot for bioregions. Increased text sizes for figures and univariate PERMANOVAS written to excel.
</commit_message>
<xml_diff>
--- a/Tables/UNI_PERM_Biomass_Boxplot.xlsx
+++ b/Tables/UNI_PERM_Biomass_Boxplot.xlsx
@@ -386,19 +386,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7.34768293483518</v>
+        <v>0.122138312895883</v>
       </c>
       <c r="C2" t="n">
-        <v>7.34768293483518</v>
+        <v>0.122138312895883</v>
       </c>
       <c r="D2" t="n">
-        <v>7.05295823772512</v>
+        <v>0.117239193324036</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0465828837782763</v>
+        <v>0.00077433319931779</v>
       </c>
       <c r="F2" t="n">
-        <v>0.009</v>
+        <v>0.7322</v>
       </c>
     </row>
     <row r="3">
@@ -406,19 +406,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.122138312895876</v>
+        <v>7.34768293483517</v>
       </c>
       <c r="C3" t="n">
-        <v>0.122138312895876</v>
+        <v>7.34768293483517</v>
       </c>
       <c r="D3" t="n">
-        <v>0.11723919332403</v>
+        <v>7.05295823772511</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000774333199317747</v>
+        <v>0.0465828837782763</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7304</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="4">
@@ -426,19 +426,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.246330117500341</v>
+        <v>0.246330117500345</v>
       </c>
       <c r="C4" t="n">
-        <v>0.246330117500341</v>
+        <v>0.246330117500345</v>
       </c>
       <c r="D4" t="n">
-        <v>0.236449510251329</v>
+        <v>0.236449510251333</v>
       </c>
       <c r="E4" t="n">
-        <v>0.001561685137529</v>
+        <v>0.00156168513752902</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6368</v>
+        <v>0.6317</v>
       </c>
     </row>
     <row r="5">

</xml_diff>